<commit_message>
Just some results from de modified codes
</commit_message>
<xml_diff>
--- a/MODIS_AOD modified/statistics_huancayo3x3.xlsx
+++ b/MODIS_AOD modified/statistics_huancayo3x3.xlsx
@@ -424,7 +424,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.38484803637325</v>
+        <v>0.2954342378901791</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -551,19 +551,19 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>0.6039024842363405</v>
+        <v>1.655896483460473</v>
       </c>
       <c r="F3">
-        <v>1.238214890565638</v>
+        <v>0.8076142579283497</v>
       </c>
       <c r="G3">
-        <v>-1.848768925569247</v>
+        <v>-0.540900480405952</v>
       </c>
       <c r="H3">
-        <v>4.239154101330603</v>
+        <v>0.2358961189181862</v>
       </c>
       <c r="I3">
-        <v>-3.063831861888978</v>
+        <v>-0.3263886678766575</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -729,13 +729,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.493596368587339</v>
+        <v>0.2862379893085237</v>
       </c>
       <c r="C3">
-        <v>4.069991605263596</v>
+        <v>0.2457007524798652</v>
       </c>
       <c r="D3">
-        <v>2.11988630354472</v>
+        <v>0.4717234119244378</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>